<commit_message>
Move all new files
</commit_message>
<xml_diff>
--- a/SeleniumTraining/data/ReadData.xlsx
+++ b/SeleniumTraining/data/ReadData.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamun\eclipse-workspace\SeleniumTraining\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamun\git\repository\SeleniumTraining\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931F3A03-4633-43CF-B081-FD77BE699A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915FC12B-88A5-43F0-8642-ECFEFEE8BF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CreatLeadData" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Example" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Cname</t>
   </si>
@@ -55,37 +55,52 @@
     <t>Helal</t>
   </si>
   <si>
-    <t>Mohd.</t>
+    <t>Mahbub</t>
+  </si>
+  <si>
+    <t>Kabir</t>
+  </si>
+  <si>
+    <t>Moriom</t>
+  </si>
+  <si>
+    <t>Akter</t>
+  </si>
+  <si>
+    <t>Sumayla</t>
+  </si>
+  <si>
+    <t>Choudhury</t>
+  </si>
+  <si>
+    <t>Mamun</t>
+  </si>
+  <si>
+    <t>Nilufar</t>
+  </si>
+  <si>
+    <t>Chowdhury</t>
+  </si>
+  <si>
+    <t>Neepa</t>
+  </si>
+  <si>
+    <t>Khan</t>
+  </si>
+  <si>
+    <t>Mahbuba</t>
+  </si>
+  <si>
+    <t>Sultana</t>
+  </si>
+  <si>
+    <t>Harun</t>
   </si>
   <si>
     <t>Shakil</t>
   </si>
   <si>
-    <t>Mahbub</t>
-  </si>
-  <si>
-    <t>Kabir</t>
-  </si>
-  <si>
-    <t>Moriom</t>
-  </si>
-  <si>
-    <t>Akter</t>
-  </si>
-  <si>
-    <t>Sumayla</t>
-  </si>
-  <si>
-    <t>Choudhury</t>
-  </si>
-  <si>
-    <t>Mamun</t>
-  </si>
-  <si>
-    <t>Nilufar</t>
-  </si>
-  <si>
-    <t>Chowdhury</t>
+    <t>Ahmed</t>
   </si>
 </sst>
 </file>
@@ -444,10 +459,13 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -465,10 +483,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -479,10 +497,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -490,10 +508,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -501,10 +519,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -531,10 +549,10 @@
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -542,10 +560,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -553,10 +571,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -564,10 +582,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -586,10 +604,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>